<commit_message>
All ID's updated complete
</commit_message>
<xml_diff>
--- a/All_IDs.xlsx
+++ b/All_IDs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliza\Desktop\ASC_small\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nask.man.ac.uk\home$\Desktop\ASC_small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B192017E-DF54-4E57-A2B3-5C7B59B45AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,7 +511,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -702,6 +701,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,24 +1015,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CO85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="18" customWidth="1"/>
-    <col min="3" max="4" width="9.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="29" customWidth="1"/>
     <col min="8" max="22" width="25.7109375" customWidth="1"/>
     <col min="23" max="23" width="25.7109375" style="26" customWidth="1"/>
     <col min="24" max="24" width="25.7109375" customWidth="1"/>
@@ -1058,10 +1059,10 @@
       <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="4" t="s">
         <v>155</v>
       </c>
       <c r="F1" s="17" t="s">
@@ -1339,10 +1340,15 @@
       <c r="C2" s="10">
         <v>37</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="E2">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F2" s="18">
+        <v>100</v>
+      </c>
       <c r="G2">
         <v>124</v>
       </c>
@@ -1619,10 +1625,15 @@
       <c r="C3" s="10">
         <v>38</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="18"/>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3" s="18">
+        <v>100</v>
+      </c>
       <c r="G3">
         <v>82</v>
       </c>
@@ -1899,10 +1910,15 @@
       <c r="C4" s="10">
         <v>47</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="E4">
+        <v>75</v>
+      </c>
+      <c r="F4" s="18">
+        <v>90</v>
+      </c>
       <c r="G4">
         <v>54</v>
       </c>
@@ -2179,10 +2195,15 @@
       <c r="C5" s="10">
         <v>25</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="E5">
+        <v>75</v>
+      </c>
+      <c r="F5" s="18">
+        <v>100</v>
+      </c>
       <c r="G5">
         <v>123</v>
       </c>
@@ -2459,10 +2480,15 @@
       <c r="C6" s="10">
         <v>46</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="E6">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F6" s="18">
+        <v>100</v>
+      </c>
       <c r="G6">
         <v>89</v>
       </c>
@@ -2739,10 +2765,15 @@
       <c r="C7" s="10">
         <v>41</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7" s="18">
+        <v>100</v>
+      </c>
       <c r="G7">
         <v>146</v>
       </c>
@@ -3019,10 +3050,15 @@
       <c r="C8" s="10">
         <v>33</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="E8">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F8" s="18">
+        <v>100</v>
+      </c>
       <c r="G8">
         <v>129</v>
       </c>
@@ -3299,10 +3335,15 @@
       <c r="C9" s="10">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="E9">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F9" s="18">
+        <v>90</v>
+      </c>
       <c r="G9">
         <v>80</v>
       </c>
@@ -3579,10 +3620,15 @@
       <c r="C10" s="10">
         <v>26</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="E10">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F10" s="18">
+        <v>90</v>
+      </c>
       <c r="G10">
         <v>113</v>
       </c>
@@ -3859,10 +3905,15 @@
       <c r="C11" s="10">
         <v>35</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="E11">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F11" s="18">
+        <v>100</v>
+      </c>
       <c r="G11">
         <v>99</v>
       </c>
@@ -4139,10 +4190,15 @@
       <c r="C12" s="10">
         <v>31</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="E12">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F12" s="18">
+        <v>100</v>
+      </c>
       <c r="G12">
         <v>101</v>
       </c>
@@ -4419,10 +4475,15 @@
       <c r="C13" s="10">
         <v>30</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="E13">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F13" s="18">
+        <v>100</v>
+      </c>
       <c r="G13">
         <v>61</v>
       </c>
@@ -4699,10 +4760,15 @@
       <c r="C14" s="10">
         <v>46</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="E14">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F14" s="18">
+        <v>100</v>
+      </c>
       <c r="G14">
         <v>125</v>
       </c>
@@ -4979,10 +5045,15 @@
       <c r="C15" s="10">
         <v>22</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="E15">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F15" s="18">
+        <v>100</v>
+      </c>
       <c r="G15">
         <v>89</v>
       </c>
@@ -5259,10 +5330,15 @@
       <c r="C16" s="10">
         <v>42</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="E16">
+        <v>75</v>
+      </c>
+      <c r="F16" s="18">
+        <v>100</v>
+      </c>
       <c r="G16">
         <v>124</v>
       </c>
@@ -5539,10 +5615,15 @@
       <c r="C17" s="10">
         <v>43</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="E17">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F17" s="18">
+        <v>90</v>
+      </c>
       <c r="G17">
         <v>100</v>
       </c>
@@ -5819,10 +5900,15 @@
       <c r="C18" s="10">
         <v>39</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="E18">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F18" s="18">
+        <v>100</v>
+      </c>
       <c r="G18">
         <v>98</v>
       </c>
@@ -6099,10 +6185,15 @@
       <c r="C19" s="10">
         <v>40</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="E19">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F19" s="18">
+        <v>100</v>
+      </c>
       <c r="G19">
         <v>97</v>
       </c>
@@ -6379,10 +6470,15 @@
       <c r="C20" s="10">
         <v>46</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="E20">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F20" s="18">
+        <v>80</v>
+      </c>
       <c r="G20">
         <v>112</v>
       </c>
@@ -6659,10 +6755,15 @@
       <c r="C21" s="10">
         <v>42</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="E21">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F21" s="18">
+        <v>100</v>
+      </c>
       <c r="G21">
         <v>95</v>
       </c>
@@ -6939,10 +7040,15 @@
       <c r="C22" s="10">
         <v>39</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="18"/>
+      <c r="E22">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F22" s="18">
+        <v>90</v>
+      </c>
       <c r="G22">
         <v>119</v>
       </c>
@@ -7219,10 +7325,15 @@
       <c r="C23" s="10">
         <v>37</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="E23">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F23" s="18">
+        <v>90</v>
+      </c>
       <c r="G23">
         <v>96</v>
       </c>
@@ -7499,10 +7610,15 @@
       <c r="C24" s="10">
         <v>41</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="18"/>
+      <c r="E24">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F24" s="18">
+        <v>100</v>
+      </c>
       <c r="G24">
         <v>149</v>
       </c>
@@ -7779,10 +7895,15 @@
       <c r="C25" s="10">
         <v>47</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="E25">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F25" s="18">
+        <v>100</v>
+      </c>
       <c r="G25">
         <v>102</v>
       </c>
@@ -8059,10 +8180,15 @@
       <c r="C26" s="10">
         <v>35</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="E26">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F26" s="18">
+        <v>100</v>
+      </c>
       <c r="G26">
         <v>99</v>
       </c>
@@ -8339,10 +8465,15 @@
       <c r="C27" s="10">
         <v>31</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="E27">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F27" s="18">
+        <v>90</v>
+      </c>
       <c r="G27">
         <v>74</v>
       </c>
@@ -8619,10 +8750,15 @@
       <c r="C28" s="10">
         <v>27</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="18"/>
+      <c r="E28">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F28" s="18">
+        <v>100</v>
+      </c>
       <c r="G28">
         <v>84</v>
       </c>
@@ -8899,10 +9035,15 @@
       <c r="C29" s="10">
         <v>28</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="E29">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F29" s="18">
+        <v>80</v>
+      </c>
       <c r="G29">
         <v>111</v>
       </c>
@@ -9179,10 +9320,15 @@
       <c r="C30" s="10">
         <v>30</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="E30">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F30" s="18">
+        <v>100</v>
+      </c>
       <c r="G30">
         <v>131</v>
       </c>
@@ -9459,11 +9605,15 @@
       <c r="C31" s="13">
         <v>21</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="19"/>
+      <c r="E31" s="13">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F31" s="19">
+        <v>100</v>
+      </c>
       <c r="G31" s="12">
         <v>126</v>
       </c>
@@ -9740,10 +9890,15 @@
       <c r="C32" s="10">
         <v>22</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F32" s="18"/>
+      <c r="E32">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F32" s="18">
+        <v>100</v>
+      </c>
       <c r="G32">
         <v>51</v>
       </c>
@@ -10020,10 +10175,15 @@
       <c r="C33" s="10">
         <v>38</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="18"/>
+      <c r="E33">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F33" s="18">
+        <v>80</v>
+      </c>
       <c r="G33">
         <v>33</v>
       </c>
@@ -10300,10 +10460,15 @@
       <c r="C34" s="10">
         <v>27</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="18"/>
+      <c r="E34">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F34" s="18">
+        <v>100</v>
+      </c>
       <c r="G34">
         <v>25</v>
       </c>
@@ -10580,10 +10745,15 @@
       <c r="C35" s="10">
         <v>49</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="18"/>
+      <c r="E35">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F35" s="18">
+        <v>100</v>
+      </c>
       <c r="G35">
         <v>36</v>
       </c>
@@ -10860,10 +11030,15 @@
       <c r="C36" s="10">
         <v>36</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="18"/>
+      <c r="E36">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F36" s="18">
+        <v>70</v>
+      </c>
       <c r="G36">
         <v>34</v>
       </c>
@@ -11140,10 +11315,15 @@
       <c r="C37" s="10">
         <v>38</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="18"/>
+      <c r="E37">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F37" s="18">
+        <v>70</v>
+      </c>
       <c r="G37">
         <v>28</v>
       </c>
@@ -11420,10 +11600,15 @@
       <c r="C38" s="10">
         <v>27</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="18"/>
+      <c r="E38">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F38" s="18">
+        <v>100</v>
+      </c>
       <c r="G38">
         <v>68</v>
       </c>
@@ -11700,10 +11885,15 @@
       <c r="C39" s="10">
         <v>22</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="18"/>
+      <c r="E39">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F39" s="18">
+        <v>90</v>
+      </c>
       <c r="G39">
         <v>71</v>
       </c>
@@ -11980,10 +12170,15 @@
       <c r="C40" s="10">
         <v>39</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="18"/>
+      <c r="E40">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F40" s="18">
+        <v>100</v>
+      </c>
       <c r="G40">
         <v>45</v>
       </c>
@@ -12260,10 +12455,15 @@
       <c r="C41" s="10">
         <v>32</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F41" s="18"/>
+      <c r="E41">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F41" s="18">
+        <v>60</v>
+      </c>
       <c r="G41">
         <v>27</v>
       </c>
@@ -12540,10 +12740,10 @@
       <c r="C42" s="10">
         <v>43</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F42" s="18"/>
+      <c r="E42"/>
       <c r="G42"/>
       <c r="K42">
         <v>4</v>
@@ -12770,10 +12970,15 @@
       <c r="C43" s="10">
         <v>27</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="18"/>
+      <c r="E43">
+        <v>75</v>
+      </c>
+      <c r="F43" s="18">
+        <v>100</v>
+      </c>
       <c r="G43">
         <v>24</v>
       </c>
@@ -13050,10 +13255,15 @@
       <c r="C44" s="10">
         <v>27</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="18"/>
+      <c r="E44">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F44" s="18">
+        <v>100</v>
+      </c>
       <c r="G44">
         <v>50</v>
       </c>
@@ -13330,10 +13540,15 @@
       <c r="C45" s="10">
         <v>34</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F45" s="18"/>
+      <c r="E45">
+        <v>75</v>
+      </c>
+      <c r="F45" s="18">
+        <v>80</v>
+      </c>
       <c r="G45">
         <v>23</v>
       </c>
@@ -13610,10 +13825,15 @@
       <c r="C46" s="10">
         <v>28</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="18"/>
+      <c r="E46">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F46" s="18">
+        <v>100</v>
+      </c>
       <c r="G46">
         <v>42</v>
       </c>
@@ -13890,10 +14110,15 @@
       <c r="C47" s="10">
         <v>33</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F47" s="18"/>
+      <c r="E47">
+        <v>75</v>
+      </c>
+      <c r="F47" s="18">
+        <v>90</v>
+      </c>
       <c r="G47">
         <v>26</v>
       </c>
@@ -14170,10 +14395,15 @@
       <c r="C48" s="10">
         <v>28</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F48" s="18"/>
+      <c r="E48">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F48" s="18">
+        <v>100</v>
+      </c>
       <c r="G48">
         <v>35</v>
       </c>
@@ -14450,10 +14680,15 @@
       <c r="C49" s="10">
         <v>30</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="18"/>
+      <c r="E49">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F49" s="18">
+        <v>100</v>
+      </c>
       <c r="G49">
         <v>41</v>
       </c>
@@ -14730,10 +14965,15 @@
       <c r="C50" s="10">
         <v>32</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F50" s="18"/>
+      <c r="E50">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F50" s="18">
+        <v>100</v>
+      </c>
       <c r="G50">
         <v>19</v>
       </c>
@@ -15010,10 +15250,15 @@
       <c r="C51" s="10">
         <v>48</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F51" s="18"/>
+      <c r="E51">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="F51" s="18">
+        <v>100</v>
+      </c>
       <c r="G51">
         <v>27</v>
       </c>
@@ -15290,10 +15535,15 @@
       <c r="C52" s="10">
         <v>38</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F52" s="18"/>
+      <c r="E52">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F52" s="18">
+        <v>100</v>
+      </c>
       <c r="G52">
         <v>18</v>
       </c>
@@ -15570,10 +15820,15 @@
       <c r="C53" s="10">
         <v>24</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F53" s="18"/>
+      <c r="E53">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F53" s="18">
+        <v>90</v>
+      </c>
       <c r="G53">
         <v>46</v>
       </c>
@@ -15850,10 +16105,15 @@
       <c r="C54" s="10">
         <v>19</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F54" s="18"/>
+      <c r="E54">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F54" s="18">
+        <v>90</v>
+      </c>
       <c r="G54">
         <v>42</v>
       </c>
@@ -16130,10 +16390,15 @@
       <c r="C55" s="10">
         <v>19</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F55" s="18"/>
+      <c r="E55">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F55" s="18">
+        <v>100</v>
+      </c>
       <c r="G55">
         <v>27</v>
       </c>
@@ -16410,10 +16675,15 @@
       <c r="C56" s="10">
         <v>20</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F56" s="18"/>
+      <c r="E56">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F56" s="18">
+        <v>100</v>
+      </c>
       <c r="G56">
         <v>34</v>
       </c>
@@ -16690,10 +16960,15 @@
       <c r="C57" s="10">
         <v>20</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F57" s="18"/>
+      <c r="E57">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F57" s="18">
+        <v>100</v>
+      </c>
       <c r="G57">
         <v>68</v>
       </c>
@@ -16970,10 +17245,15 @@
       <c r="C58" s="10">
         <v>20</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F58" s="18"/>
+      <c r="E58">
+        <v>91.6666666666667</v>
+      </c>
+      <c r="F58" s="18">
+        <v>100</v>
+      </c>
       <c r="G58">
         <v>56</v>
       </c>
@@ -17250,10 +17530,15 @@
       <c r="C59" s="10">
         <v>19</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F59" s="18"/>
+      <c r="E59">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F59" s="18">
+        <v>90</v>
+      </c>
       <c r="G59">
         <v>68</v>
       </c>
@@ -17530,10 +17815,15 @@
       <c r="C60" s="10">
         <v>40</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F60" s="18"/>
+      <c r="E60">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F60" s="18">
+        <v>90</v>
+      </c>
       <c r="G60">
         <v>76</v>
       </c>
@@ -17810,10 +18100,15 @@
       <c r="C61" s="10">
         <v>43</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F61" s="18"/>
+      <c r="E61">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="F61" s="18">
+        <v>90</v>
+      </c>
       <c r="G61">
         <v>57</v>
       </c>

</xml_diff>